<commit_message>
`Refactor delivery note template: update header and signature positions`
</commit_message>
<xml_diff>
--- a/assets/template.xlsx
+++ b/assets/template.xlsx
@@ -2,66 +2,54 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/codeemperor/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6943D242-DA96-1A4A-A991-01ACCE40247A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DF2FD6C-E721-5B42-B558-0B3A9A736B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{46EDE84F-B0C5-D142-99EE-322EC255F680}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Delivery Note" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>LOGO</t>
-  </si>
-  <si>
-    <t>Umayumcha Head Quarter</t>
-  </si>
-  <si>
-    <t>Jalan Dirgantara 4 no A5/11</t>
-  </si>
-  <si>
-    <t>Sawojajar Malang</t>
-  </si>
-  <si>
-    <t>No. Surat Jalan</t>
-  </si>
-  <si>
-    <t>Kepada</t>
-  </si>
-  <si>
-    <t>Tanggal</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+  <si>
+    <t>No. Surat Jalan:</t>
+  </si>
+  <si>
+    <t>GA/08/2025/0023</t>
+  </si>
+  <si>
+    <t>Penerima:</t>
+  </si>
+  <si>
+    <t>Cabang HQ JOGJA</t>
+  </si>
+  <si>
+    <t>Tanggal:</t>
+  </si>
+  <si>
+    <t>03-08-2025</t>
+  </si>
+  <si>
+    <t>Catatan:</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>Nama Barang</t>
   </si>
   <si>
-    <t>QTY</t>
+    <t>Quantity</t>
   </si>
   <si>
     <t>Check</t>
@@ -70,23 +58,58 @@
     <t>Keterangan</t>
   </si>
   <si>
+    <t>Meja Makan</t>
+  </si>
+  <si>
+    <t>✓</t>
+  </si>
+  <si>
     <t>Pengirim</t>
   </si>
   <si>
     <t>Penerima</t>
+  </si>
+  <si>
+    <t>(____________)</t>
+  </si>
+  <si>
+    <t>Mengetahui</t>
+  </si>
+  <si>
+    <t>HEADQUARTERS</t>
+  </si>
+  <si>
+    <t>MALANG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -121,17 +144,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="headerStyle" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -145,6 +173,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1428750" cy="476250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -443,131 +520,139 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95EDF9A-1418-C14F-AA85-24D66D9DA201}">
-  <dimension ref="A1:D20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="2" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4">
+        <v>5</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-  </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>